<commit_message>
source data for figure 2
</commit_message>
<xml_diff>
--- a/figure2.xlsx
+++ b/figure2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/TakumaWatari/Dropbox/GitHub/concrete-flows-global/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEA14951-3150-BE42-B8BF-EB9BB284C9B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCCA26B9-826B-9244-98FE-7378FCF1390B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1040" yWindow="-19220" windowWidth="27500" windowHeight="16440" xr2:uid="{2B4E0CDE-24E4-BC4C-9492-0837B10339EB}"/>
   </bookViews>
@@ -37,13 +37,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>Fossil fuels</t>
-  </si>
-  <si>
-    <t>mean</t>
-    <phoneticPr fontId="2"/>
   </si>
 </sst>
 </file>
@@ -849,735 +845,1047 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C44B7409-72A9-2440-B1AB-E7F356E2FF1D}">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:F52"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <sheetData>
-    <row r="1" spans="1:4">
-      <c r="B1" t="s">
-        <v>1</v>
+    <row r="1" spans="1:6">
+      <c r="B1">
+        <v>0.05</v>
       </c>
       <c r="C1" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D1" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="E1">
+        <v>0.75</v>
+      </c>
+      <c r="F1">
         <v>0.95</v>
       </c>
-      <c r="D1" s="2">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1970</v>
       </c>
       <c r="B2" s="1">
-        <v>2717.292075930975</v>
+        <v>2297.4925164302122</v>
       </c>
       <c r="C2" s="1">
-        <v>3198.585222125223</v>
+        <v>2498.5813566263569</v>
       </c>
       <c r="D2" s="1">
-        <v>2266.2882028869899</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+        <v>2672.5171517662102</v>
+      </c>
+      <c r="E2" s="1">
+        <v>2866.9240661357671</v>
+      </c>
+      <c r="F2" s="1">
+        <v>3093.18801288029</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>1971</v>
       </c>
       <c r="B3" s="1">
-        <v>2804.8689157090348</v>
+        <v>2371.4644431178208</v>
       </c>
       <c r="C3" s="1">
-        <v>3301.5323595032451</v>
+        <v>2578.9390590816788</v>
       </c>
       <c r="D3" s="1">
-        <v>2339.2970984196568</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+        <v>2758.8843858375012</v>
+      </c>
+      <c r="E3" s="1">
+        <v>2959.5721986944832</v>
+      </c>
+      <c r="F3" s="1">
+        <v>3192.8152269732359</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>1972</v>
       </c>
       <c r="B4" s="1">
-        <v>3140.3985104251328</v>
+        <v>2655.2867527088129</v>
       </c>
       <c r="C4" s="1">
-        <v>3696.7357349693611</v>
+        <v>2887.8086316242711</v>
       </c>
       <c r="D4" s="1">
-        <v>2619.076157204086</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+        <v>3088.4826795596482</v>
+      </c>
+      <c r="E4" s="1">
+        <v>3313.2112283628771</v>
+      </c>
+      <c r="F4" s="1">
+        <v>3574.9020595068728</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>1973</v>
       </c>
       <c r="B5" s="1">
-        <v>3334.4590777712201</v>
+        <v>2819.4202389438101</v>
       </c>
       <c r="C5" s="1">
-        <v>3925.2700896521128</v>
+        <v>3066.4236189055209</v>
       </c>
       <c r="D5" s="1">
-        <v>2780.8838501459841</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+        <v>3279.1784030034819</v>
+      </c>
+      <c r="E5" s="1">
+        <v>3517.9904099620712</v>
+      </c>
+      <c r="F5" s="1">
+        <v>3795.8843676216839</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>1974</v>
       </c>
       <c r="B6" s="1">
-        <v>3338.8448705985029</v>
+        <v>2823.2192964601732</v>
       </c>
       <c r="C6" s="1">
-        <v>3930.6040936359241</v>
+        <v>3070.7787501285538</v>
       </c>
       <c r="D6" s="1">
-        <v>2784.8494958672331</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+        <v>3283.2960518233149</v>
+      </c>
+      <c r="E6" s="1">
+        <v>3522.5569350566388</v>
+      </c>
+      <c r="F6" s="1">
+        <v>3801.006130784916</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>1975</v>
       </c>
       <c r="B7" s="1">
-        <v>3330.355703266956</v>
+        <v>2816.1954280502891</v>
       </c>
       <c r="C7" s="1">
-        <v>3921.097691795806</v>
+        <v>3063.868975875956</v>
       </c>
       <c r="D7" s="1">
-        <v>2778.6459545405019</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+        <v>3275.3224839486561</v>
+      </c>
+      <c r="E7" s="1">
+        <v>3514.456711815345</v>
+      </c>
+      <c r="F7" s="1">
+        <v>3791.709452225542</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>1976</v>
       </c>
       <c r="B8" s="1">
-        <v>3487.2172742088701</v>
+        <v>2948.7557583043699</v>
       </c>
       <c r="C8" s="1">
-        <v>4105.8614638793761</v>
+        <v>3208.4353826797251</v>
       </c>
       <c r="D8" s="1">
-        <v>2909.661947934329</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+        <v>3429.7812157072121</v>
+      </c>
+      <c r="E8" s="1">
+        <v>3679.8747692940228</v>
+      </c>
+      <c r="F8" s="1">
+        <v>3970.3598125987678</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>1977</v>
       </c>
       <c r="B9" s="1">
-        <v>3779.4927026508931</v>
+        <v>3195.8584740201341</v>
       </c>
       <c r="C9" s="1">
-        <v>4450.0269136963161</v>
+        <v>3477.4747378495449</v>
       </c>
       <c r="D9" s="1">
-        <v>3153.601368506434</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+        <v>3717.3383386201749</v>
+      </c>
+      <c r="E9" s="1">
+        <v>3988.2254032001879</v>
+      </c>
+      <c r="F9" s="1">
+        <v>4303.1587361821257</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>1978</v>
       </c>
       <c r="B10" s="1">
-        <v>4044.264538323926</v>
+        <v>3419.704375158914</v>
       </c>
       <c r="C10" s="1">
-        <v>4761.8095899694163</v>
+        <v>3721.2094104340658</v>
       </c>
       <c r="D10" s="1">
-        <v>3374.592450277768</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+        <v>3977.8449869151609</v>
+      </c>
+      <c r="E10" s="1">
+        <v>4267.5848141830966</v>
+      </c>
+      <c r="F10" s="1">
+        <v>4604.6435719621131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>1979</v>
       </c>
       <c r="B11" s="1">
-        <v>4135.5544046148734</v>
+        <v>3496.7992270918521</v>
       </c>
       <c r="C11" s="1">
-        <v>4869.3863666309098</v>
+        <v>3805.5032874496178</v>
       </c>
       <c r="D11" s="1">
-        <v>3450.927998956362</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+        <v>4067.8541500568499</v>
+      </c>
+      <c r="E11" s="1">
+        <v>4364.0254474830381</v>
+      </c>
+      <c r="F11" s="1">
+        <v>4708.6505698990377</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>1980</v>
       </c>
       <c r="B12" s="1">
-        <v>4183.1644697459469</v>
+        <v>3536.6178977040681</v>
       </c>
       <c r="C12" s="1">
-        <v>4925.8507015558253</v>
+        <v>3850.1663736303012</v>
       </c>
       <c r="D12" s="1">
-        <v>3491.3872785907638</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+        <v>4115.45121420544</v>
+      </c>
+      <c r="E12" s="1">
+        <v>4414.7324344297931</v>
+      </c>
+      <c r="F12" s="1">
+        <v>4763.1646318946077</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>1981</v>
       </c>
       <c r="B13" s="1">
-        <v>4199.5494791672354</v>
+        <v>3550.376443974998</v>
       </c>
       <c r="C13" s="1">
-        <v>4945.2319393258294</v>
+        <v>3865.5041786265701</v>
       </c>
       <c r="D13" s="1">
-        <v>3505.2196143019341</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+        <v>4131.6073752055763</v>
+      </c>
+      <c r="E13" s="1">
+        <v>4432.1231890293548</v>
+      </c>
+      <c r="F13" s="1">
+        <v>4781.8872110507618</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>1982</v>
       </c>
       <c r="B14" s="1">
-        <v>4200.135289364327</v>
+        <v>3550.4874306164202</v>
       </c>
       <c r="C14" s="1">
-        <v>4946.278225378991</v>
+        <v>3866.3680741734529</v>
       </c>
       <c r="D14" s="1">
-        <v>3506.3500874358028</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4">
+        <v>4132.3377294385973</v>
+      </c>
+      <c r="E14" s="1">
+        <v>4433.144958208899</v>
+      </c>
+      <c r="F14" s="1">
+        <v>4782.8230962536036</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>1983</v>
       </c>
       <c r="B15" s="1">
-        <v>4339.2554744608487</v>
+        <v>3668.218262557833</v>
       </c>
       <c r="C15" s="1">
-        <v>5109.9932705515093</v>
+        <v>3994.4075908545519</v>
       </c>
       <c r="D15" s="1">
-        <v>3622.2751573318251</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4">
+        <v>4269.156928982643</v>
+      </c>
+      <c r="E15" s="1">
+        <v>4579.8478271564973</v>
+      </c>
+      <c r="F15" s="1">
+        <v>4941.1534178829779</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="A16">
         <v>1984</v>
       </c>
       <c r="B16" s="1">
-        <v>4456.3489708644302</v>
+        <v>3767.3601632790401</v>
       </c>
       <c r="C16" s="1">
-        <v>5247.7400529011402</v>
+        <v>4102.1647169848566</v>
       </c>
       <c r="D16" s="1">
-        <v>3719.760487533958</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4">
+        <v>4384.2984181908341</v>
+      </c>
+      <c r="E16" s="1">
+        <v>4703.2696736932294</v>
+      </c>
+      <c r="F16" s="1">
+        <v>5074.3797088026586</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
       <c r="A17">
         <v>1985</v>
       </c>
       <c r="B17" s="1">
-        <v>4541.9144281747986</v>
+        <v>3839.5430420758489</v>
       </c>
       <c r="C17" s="1">
-        <v>5348.6431891644361</v>
+        <v>4180.9597771291601</v>
       </c>
       <c r="D17" s="1">
-        <v>3791.4390246503121</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4">
+        <v>4468.5398228970998</v>
+      </c>
+      <c r="E17" s="1">
+        <v>4793.7373351764336</v>
+      </c>
+      <c r="F17" s="1">
+        <v>5171.9192021018816</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
       <c r="A18">
         <v>1986</v>
       </c>
       <c r="B18" s="1">
-        <v>4770.7521814791726</v>
+        <v>4032.8181227695791</v>
       </c>
       <c r="C18" s="1">
-        <v>5618.2888654580865</v>
+        <v>4391.645767627544</v>
       </c>
       <c r="D18" s="1">
-        <v>3982.7568392045068</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4">
+        <v>4693.7664641598631</v>
+      </c>
+      <c r="E18" s="1">
+        <v>5035.4462826705558</v>
+      </c>
+      <c r="F18" s="1">
+        <v>5432.6210620366392</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
       <c r="A19">
         <v>1987</v>
       </c>
       <c r="B19" s="1">
-        <v>4982.2376149517549</v>
+        <v>4211.3806939361057</v>
       </c>
       <c r="C19" s="1">
-        <v>5867.5405610829703</v>
+        <v>4586.3670461319389</v>
       </c>
       <c r="D19" s="1">
-        <v>4159.6622854482284</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4">
+        <v>4902.2166211622934</v>
+      </c>
+      <c r="E19" s="1">
+        <v>5258.8865975672652</v>
+      </c>
+      <c r="F19" s="1">
+        <v>5673.5941741093466</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
       <c r="A20">
         <v>1988</v>
       </c>
       <c r="B20" s="1">
-        <v>5287.6382347252929</v>
+        <v>4469.2271491040729</v>
       </c>
       <c r="C20" s="1">
-        <v>6227.488768963336</v>
+        <v>4867.5611744642401</v>
       </c>
       <c r="D20" s="1">
-        <v>4415.1453992956749</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4">
+        <v>5203.4188741772195</v>
+      </c>
+      <c r="E20" s="1">
+        <v>5581.78736069556</v>
+      </c>
+      <c r="F20" s="1">
+        <v>6021.5508737487171</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
       <c r="A21">
         <v>1989</v>
       </c>
       <c r="B21" s="1">
-        <v>5435.2204206811311</v>
+        <v>4594.1030317645982</v>
       </c>
       <c r="C21" s="1">
-        <v>6401.1765868236562</v>
+        <v>5003.3918488177806</v>
       </c>
       <c r="D21" s="1">
-        <v>4538.1482362091638</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4">
+        <v>5348.3319710843443</v>
+      </c>
+      <c r="E21" s="1">
+        <v>5737.2760831492396</v>
+      </c>
+      <c r="F21" s="1">
+        <v>6189.5383702641757</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
       <c r="A22">
         <v>1990</v>
       </c>
       <c r="B22" s="1">
-        <v>5487.4636981559152</v>
+        <v>4638.290953064231</v>
       </c>
       <c r="C22" s="1">
-        <v>6462.6773010815514</v>
+        <v>5051.4785933349067</v>
       </c>
       <c r="D22" s="1">
-        <v>4581.7196927212126</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4">
+        <v>5399.6712077681887</v>
+      </c>
+      <c r="E22" s="1">
+        <v>5792.3571032030559</v>
+      </c>
+      <c r="F22" s="1">
+        <v>6249.0151076222865</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6">
       <c r="A23">
         <v>1991</v>
       </c>
       <c r="B23" s="1">
-        <v>5586.9089715075079</v>
+        <v>4721.6950747383889</v>
       </c>
       <c r="C23" s="1">
-        <v>6580.4006698519152</v>
+        <v>5143.4968042389337</v>
       </c>
       <c r="D23" s="1">
-        <v>4665.8396798702852</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4">
+        <v>5499.0504764736206</v>
+      </c>
+      <c r="E23" s="1">
+        <v>5897.6797138254433</v>
+      </c>
+      <c r="F23" s="1">
+        <v>6362.6386418625034</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
       <c r="A24">
         <v>1992</v>
       </c>
       <c r="B24" s="1">
-        <v>5817.376867633996</v>
+        <v>4916.3110963850349</v>
       </c>
       <c r="C24" s="1">
-        <v>6852.0004599031736</v>
+        <v>5356.0571508950143</v>
       </c>
       <c r="D24" s="1">
-        <v>4858.5802419614038</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4">
+        <v>5726.2695427620383</v>
+      </c>
+      <c r="E24" s="1">
+        <v>6141.1796029388825</v>
+      </c>
+      <c r="F24" s="1">
+        <v>6625.1993574531143</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
       <c r="A25">
         <v>1993</v>
       </c>
       <c r="B25" s="1">
-        <v>6098.7820352842018</v>
+        <v>5153.8270539273954</v>
       </c>
       <c r="C25" s="1">
-        <v>7183.7336179723616</v>
+        <v>5615.8921939032753</v>
       </c>
       <c r="D25" s="1">
-        <v>5094.1091344674314</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4">
+        <v>6003.3926187513043</v>
+      </c>
+      <c r="E25" s="1">
+        <v>6438.6470434111743</v>
+      </c>
+      <c r="F25" s="1">
+        <v>6945.8560238210421</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
       <c r="A26">
         <v>1994</v>
       </c>
       <c r="B26" s="1">
-        <v>6470.7292220245827</v>
+        <v>5467.9670439689826</v>
       </c>
       <c r="C26" s="1">
-        <v>7622.0131740933448</v>
+        <v>5959.028053872752</v>
       </c>
       <c r="D26" s="1">
-        <v>5405.0798829221912</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4">
+        <v>6369.5898556301818</v>
+      </c>
+      <c r="E26" s="1">
+        <v>6831.5557318281544</v>
+      </c>
+      <c r="F26" s="1">
+        <v>7369.5662528592284</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
       <c r="A27">
         <v>1995</v>
       </c>
       <c r="B27" s="1">
-        <v>6823.3012408219574</v>
+        <v>5765.666296872233</v>
       </c>
       <c r="C27" s="1">
-        <v>8037.5301865704414</v>
+        <v>6284.5665905431979</v>
       </c>
       <c r="D27" s="1">
-        <v>5699.9800359284609</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4">
+        <v>6716.6380843132056</v>
+      </c>
+      <c r="E27" s="1">
+        <v>7204.0988803073988</v>
+      </c>
+      <c r="F27" s="1">
+        <v>7771.2493431818093</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
       <c r="A28">
         <v>1996</v>
       </c>
       <c r="B28" s="1">
-        <v>7048.7702894378581</v>
+        <v>5956.3108182490687</v>
       </c>
       <c r="C28" s="1">
-        <v>8303.2636871071354</v>
+        <v>6492.7173722658927</v>
       </c>
       <c r="D28" s="1">
-        <v>5888.6099725305876</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4">
+        <v>6938.4219952421772</v>
+      </c>
+      <c r="E28" s="1">
+        <v>7442.1688741723146</v>
+      </c>
+      <c r="F28" s="1">
+        <v>8027.4295961908192</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
       <c r="A29">
         <v>1997</v>
       </c>
       <c r="B29" s="1">
-        <v>7303.7657440169987</v>
+        <v>6171.7757531735606</v>
       </c>
       <c r="C29" s="1">
-        <v>8603.6355850157452</v>
+        <v>6727.5905737705334</v>
       </c>
       <c r="D29" s="1">
-        <v>6101.6238252235726</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4">
+        <v>7189.432263140312</v>
+      </c>
+      <c r="E29" s="1">
+        <v>7711.3966268149061</v>
+      </c>
+      <c r="F29" s="1">
+        <v>8317.8553138048901</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
       <c r="A30">
         <v>1998</v>
       </c>
       <c r="B30" s="1">
-        <v>7270.2128462314759</v>
+        <v>6143.5223794368376</v>
       </c>
       <c r="C30" s="1">
-        <v>8564.1712848253937</v>
+        <v>6696.750658587307</v>
       </c>
       <c r="D30" s="1">
-        <v>6073.7123415651567</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4">
+        <v>7156.3364120129318</v>
+      </c>
+      <c r="E30" s="1">
+        <v>7675.9634513656511</v>
+      </c>
+      <c r="F30" s="1">
+        <v>8279.377417786689</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
       <c r="A31">
         <v>1999</v>
       </c>
       <c r="B31" s="1">
-        <v>7552.5392657375769</v>
+        <v>6382.2785054443029</v>
       </c>
       <c r="C31" s="1">
-        <v>8896.8570802369122</v>
+        <v>6956.9293637158626</v>
       </c>
       <c r="D31" s="1">
-        <v>6309.7936483766498</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4">
+        <v>7434.1150254444747</v>
+      </c>
+      <c r="E31" s="1">
+        <v>7974.0324091163602</v>
+      </c>
+      <c r="F31" s="1">
+        <v>8600.402420403645</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
       <c r="A32">
         <v>2000</v>
       </c>
       <c r="B32" s="1">
-        <v>7835.7162324370174</v>
+        <v>6621.5859131952666</v>
       </c>
       <c r="C32" s="1">
-        <v>9230.4434221932097</v>
+        <v>7217.7800407835111</v>
       </c>
       <c r="D32" s="1">
-        <v>6546.3849725455757</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4">
+        <v>7712.8459098290195</v>
+      </c>
+      <c r="E32" s="1">
+        <v>8273.0122977934079</v>
+      </c>
+      <c r="F32" s="1">
+        <v>8922.8453980669092</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
       <c r="A33">
         <v>2001</v>
       </c>
       <c r="B33" s="1">
-        <v>8257.63336410388</v>
+        <v>6978.7012194717672</v>
       </c>
       <c r="C33" s="1">
-        <v>9727.8071785679931</v>
+        <v>7606.805752061493</v>
       </c>
       <c r="D33" s="1">
-        <v>6898.7072146534974</v>
-      </c>
-    </row>
-    <row r="34" spans="1:4">
+        <v>8127.7532647866155</v>
+      </c>
+      <c r="E33" s="1">
+        <v>8718.4315989598235</v>
+      </c>
+      <c r="F33" s="1">
+        <v>9402.4366618706663</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
       <c r="A34">
         <v>2002</v>
       </c>
       <c r="B34" s="1">
-        <v>8727.2083942898789</v>
+        <v>7376.0644241248356</v>
       </c>
       <c r="C34" s="1">
-        <v>10281.25753920247</v>
+        <v>8040.014905373424</v>
       </c>
       <c r="D34" s="1">
-        <v>7290.8696443795334</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4">
+        <v>8589.7383878880246</v>
+      </c>
+      <c r="E34" s="1">
+        <v>9213.5637730427406</v>
+      </c>
+      <c r="F34" s="1">
+        <v>9937.2564657428829</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
       <c r="A35">
         <v>2003</v>
       </c>
       <c r="B35" s="1">
-        <v>9524.9238184603018</v>
+        <v>8051.2333317436232</v>
       </c>
       <c r="C35" s="1">
-        <v>11221.52798053422</v>
+        <v>8776.6883100832983</v>
       </c>
       <c r="D35" s="1">
-        <v>7957.0426466545223</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4">
+        <v>9375.3880822841038</v>
+      </c>
+      <c r="E35" s="1">
+        <v>10054.062464608951</v>
+      </c>
+      <c r="F35" s="1">
+        <v>10845.84564246805</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
       <c r="A36">
         <v>2004</v>
       </c>
       <c r="B36" s="1">
-        <v>10324.22168071436</v>
+        <v>8727.3834113890334</v>
       </c>
       <c r="C36" s="1">
-        <v>12163.47332934276</v>
+        <v>9514.1591389321293</v>
       </c>
       <c r="D36" s="1">
-        <v>8624.6319998821527</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4">
+        <v>10162.408944490569</v>
+      </c>
+      <c r="E36" s="1">
+        <v>10897.57625070064</v>
+      </c>
+      <c r="F36" s="1">
+        <v>11756.1365120914</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6">
       <c r="A37">
         <v>2005</v>
       </c>
       <c r="B37" s="1">
-        <v>11076.995111688329</v>
+        <v>9364.0656915809577</v>
       </c>
       <c r="C37" s="1">
-        <v>13050.528032010719</v>
+        <v>10208.49780932172</v>
       </c>
       <c r="D37" s="1">
-        <v>9253.3927281904562</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4">
+        <v>10903.56869661788</v>
+      </c>
+      <c r="E37" s="1">
+        <v>11692.03389405073</v>
+      </c>
+      <c r="F37" s="1">
+        <v>12613.4111099764</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
       <c r="A38">
         <v>2006</v>
       </c>
       <c r="B38" s="1">
-        <v>12342.86096982651</v>
+        <v>10436.298324165169</v>
       </c>
       <c r="C38" s="1">
-        <v>14542.71886900979</v>
+        <v>11377.892062801</v>
       </c>
       <c r="D38" s="1">
-        <v>10310.45308457765</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4">
+        <v>12150.74148318938</v>
+      </c>
+      <c r="E38" s="1">
+        <v>13024.86599115838</v>
+      </c>
+      <c r="F38" s="1">
+        <v>14055.22346419411</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
       <c r="A39">
         <v>2007</v>
       </c>
       <c r="B39" s="1">
-        <v>13233.6996062292</v>
+        <v>11191.205791153339</v>
       </c>
       <c r="C39" s="1">
-        <v>15592.825962516299</v>
+        <v>12200.357994494279</v>
       </c>
       <c r="D39" s="1">
-        <v>11054.349882883531</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4">
+        <v>13028.417746710589</v>
+      </c>
+      <c r="E39" s="1">
+        <v>13962.661545839819</v>
+      </c>
+      <c r="F39" s="1">
+        <v>15069.848998621181</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
       <c r="A40">
         <v>2008</v>
       </c>
       <c r="B40" s="1">
-        <v>13418.083551417451</v>
+        <v>11348.704619373701</v>
       </c>
       <c r="C40" s="1">
-        <v>15810.544531076421</v>
+        <v>12371.54093446194</v>
       </c>
       <c r="D40" s="1">
-        <v>11208.13047493782</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4">
+        <v>13210.602754460369</v>
+      </c>
+      <c r="E40" s="1">
+        <v>14155.07253700541</v>
+      </c>
+      <c r="F40" s="1">
+        <v>15280.00203615614</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
       <c r="A41">
         <v>2009</v>
       </c>
       <c r="B41" s="1">
-        <v>14345.272469772141</v>
+        <v>12138.58089151857</v>
       </c>
       <c r="C41" s="1">
-        <v>16904.732579796611</v>
+        <v>13225.59189470116</v>
       </c>
       <c r="D41" s="1">
-        <v>11981.749591734881</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4">
+        <v>14125.843358745669</v>
+      </c>
+      <c r="E41" s="1">
+        <v>15133.438193304301</v>
+      </c>
+      <c r="F41" s="1">
+        <v>16335.516668154631</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
       <c r="A42">
         <v>2010</v>
       </c>
       <c r="B42" s="1">
-        <v>15469.8500578773</v>
+        <v>13091.25154630804</v>
       </c>
       <c r="C42" s="1">
-        <v>18228.156108248939</v>
+        <v>14261.1851631182</v>
       </c>
       <c r="D42" s="1">
-        <v>12920.78909503571</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4">
+        <v>15233.86469602235</v>
+      </c>
+      <c r="E42" s="1">
+        <v>16319.45987816235</v>
+      </c>
+      <c r="F42" s="1">
+        <v>17615.33759861912</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
       <c r="A43">
         <v>2011</v>
       </c>
       <c r="B43" s="1">
-        <v>17068.84152952646</v>
+        <v>14444.36703742481</v>
       </c>
       <c r="C43" s="1">
-        <v>20112.38812692487</v>
+        <v>15735.32788454044</v>
       </c>
       <c r="D43" s="1">
-        <v>14256.32201240515</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4">
+        <v>16808.46136493636</v>
+      </c>
+      <c r="E43" s="1">
+        <v>18006.31525016854</v>
+      </c>
+      <c r="F43" s="1">
+        <v>19436.044878716501</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
       <c r="A44">
         <v>2012</v>
       </c>
       <c r="B44" s="1">
-        <v>17959.11175876515</v>
+        <v>15197.96982735482</v>
       </c>
       <c r="C44" s="1">
-        <v>21159.884477285748</v>
+        <v>16555.147966981342</v>
       </c>
       <c r="D44" s="1">
-        <v>14999.71006156214</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4">
+        <v>17685.183253395531</v>
+      </c>
+      <c r="E44" s="1">
+        <v>18944.96468252884</v>
+      </c>
+      <c r="F44" s="1">
+        <v>20450.613687341429</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
       <c r="A45">
         <v>2013</v>
       </c>
       <c r="B45" s="1">
-        <v>18942.728768996629</v>
+        <v>16030.61511481368</v>
       </c>
       <c r="C45" s="1">
-        <v>22317.029580522481</v>
+        <v>17460.82306936659</v>
       </c>
       <c r="D45" s="1">
-        <v>15821.022010520401</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4">
+        <v>18653.835146208789</v>
+      </c>
+      <c r="E45" s="1">
+        <v>19981.842064438479</v>
+      </c>
+      <c r="F45" s="1">
+        <v>21571.699286483588</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
       <c r="A46">
         <v>2014</v>
       </c>
       <c r="B46" s="1">
-        <v>19508.720818102211</v>
+        <v>16509.460438595452</v>
       </c>
       <c r="C46" s="1">
-        <v>22984.787438544328</v>
+        <v>17983.091759753661</v>
       </c>
       <c r="D46" s="1">
-        <v>16293.8563366091</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4">
+        <v>19211.175235231171</v>
+      </c>
+      <c r="E46" s="1">
+        <v>20579.270141881319</v>
+      </c>
+      <c r="F46" s="1">
+        <v>22215.707881820981</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
       <c r="A47">
         <v>2015</v>
       </c>
       <c r="B47" s="1">
-        <v>19136.693394053549</v>
+        <v>16194.346293450741</v>
       </c>
       <c r="C47" s="1">
-        <v>22548.427738036589</v>
+        <v>17641.313655576709</v>
       </c>
       <c r="D47" s="1">
-        <v>15983.37772800884</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4">
+        <v>18844.78011646829</v>
+      </c>
+      <c r="E47" s="1">
+        <v>20187.55900735965</v>
+      </c>
+      <c r="F47" s="1">
+        <v>21790.944347321001</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6">
       <c r="A48">
         <v>2016</v>
       </c>
       <c r="B48" s="1">
-        <v>19511.62578869157</v>
+        <v>16511.716229403381</v>
       </c>
       <c r="C48" s="1">
-        <v>22989.614715587191</v>
+        <v>17986.599806454939</v>
       </c>
       <c r="D48" s="1">
-        <v>16296.456411711049</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4">
+        <v>19214.005853633389</v>
+      </c>
+      <c r="E48" s="1">
+        <v>20582.879551941369</v>
+      </c>
+      <c r="F48" s="1">
+        <v>22218.21547634956</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
       <c r="A49">
         <v>2017</v>
       </c>
       <c r="B49" s="1">
-        <v>19279.54137658433</v>
+        <v>16315.10591400778</v>
       </c>
       <c r="C49" s="1">
-        <v>22717.608979781158</v>
+        <v>17773.51105421262</v>
       </c>
       <c r="D49" s="1">
-        <v>16102.794591659471</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4">
+        <v>18985.3434382831</v>
+      </c>
+      <c r="E49" s="1">
+        <v>20338.546337250951</v>
+      </c>
+      <c r="F49" s="1">
+        <v>21953.478440384599</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
       <c r="A50">
         <v>2018</v>
       </c>
       <c r="B50" s="1">
-        <v>19048.16664436692</v>
+        <v>16118.229258464849</v>
       </c>
       <c r="C50" s="1">
-        <v>22446.76468581576</v>
+        <v>17561.27931243561</v>
       </c>
       <c r="D50" s="1">
-        <v>15909.76796599459</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4">
+        <v>18756.879320332519</v>
+      </c>
+      <c r="E50" s="1">
+        <v>20094.77349565976</v>
+      </c>
+      <c r="F50" s="1">
+        <v>21690.786349188998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
       <c r="A51">
         <v>2019</v>
       </c>
       <c r="B51" s="1">
-        <v>19280.07887943435</v>
+        <v>16315.52329998502</v>
       </c>
       <c r="C51" s="1">
-        <v>22718.50216444123</v>
+        <v>17774.160143434681</v>
       </c>
       <c r="D51" s="1">
-        <v>16103.27568010239</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4">
+        <v>18985.783663006969</v>
+      </c>
+      <c r="E51" s="1">
+        <v>20339.20188932171</v>
+      </c>
+      <c r="F51" s="1">
+        <v>21954.201492134351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
       <c r="A52">
         <v>2020</v>
       </c>
       <c r="B52" s="1">
-        <v>19749.3286371426</v>
+        <v>16712.689417561171</v>
       </c>
       <c r="C52" s="1">
-        <v>23270.956776132109</v>
+        <v>18206.47339058312</v>
       </c>
       <c r="D52" s="1">
-        <v>16495.146976804968</v>
+        <v>19448.03575870032</v>
+      </c>
+      <c r="E52" s="1">
+        <v>20834.065153701769</v>
+      </c>
+      <c r="F52" s="1">
+        <v>22488.32990430039</v>
       </c>
     </row>
   </sheetData>

</xml_diff>